<commit_message>
stopping agent after 1500 steps, made some changes to configs
</commit_message>
<xml_diff>
--- a/experiment_results.xlsx
+++ b/experiment_results.xlsx
@@ -742,187 +742,187 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>37.5</v>
+        <v>130.6</v>
       </c>
       <c r="B2" t="n">
-        <v>5.835237784358063</v>
+        <v>4.176122603564219</v>
       </c>
       <c r="C2" t="n">
-        <v>34.5</v>
+        <v>135.5</v>
       </c>
       <c r="D2" t="n">
-        <v>6.756478372643548</v>
+        <v>3.640054944640259</v>
       </c>
       <c r="E2" t="n">
-        <v>29.1</v>
+        <v>132.7</v>
       </c>
       <c r="F2" t="n">
-        <v>13.39738780509096</v>
+        <v>3.950949253027682</v>
       </c>
       <c r="G2" t="n">
-        <v>20.7</v>
+        <v>131.3</v>
       </c>
       <c r="H2" t="n">
-        <v>13.73353559721603</v>
+        <v>3.226453160980336</v>
       </c>
       <c r="I2" t="n">
-        <v>19.3</v>
+        <v>131.2</v>
       </c>
       <c r="J2" t="n">
-        <v>14.12126056696073</v>
+        <v>4.019950248448356</v>
       </c>
       <c r="K2" t="n">
-        <v>10.6</v>
+        <v>134.3</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8</v>
+        <v>5.273518749374084</v>
       </c>
       <c r="M2" t="n">
-        <v>13.3</v>
+        <v>131</v>
       </c>
       <c r="N2" t="n">
-        <v>7.280796659706958</v>
+        <v>3.898717737923585</v>
       </c>
       <c r="O2" t="n">
-        <v>11.4</v>
+        <v>132.5</v>
       </c>
       <c r="P2" t="n">
-        <v>0.8</v>
+        <v>3.263433774416144</v>
       </c>
       <c r="Q2" t="n">
-        <v>11.5</v>
+        <v>128.5</v>
       </c>
       <c r="R2" t="n">
-        <v>0.9219544457292888</v>
+        <v>4.031128874149275</v>
       </c>
       <c r="S2" t="n">
-        <v>11</v>
+        <v>129.9</v>
       </c>
       <c r="T2" t="n">
-        <v>0.6324555320336759</v>
+        <v>2.3</v>
       </c>
       <c r="U2" t="n">
-        <v>11.9</v>
+        <v>125.5</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9433981132056604</v>
+        <v>3.556683848755748</v>
       </c>
       <c r="W2" t="n">
-        <v>12.6</v>
+        <v>123.9</v>
       </c>
       <c r="X2" t="n">
-        <v>1.113552872566004</v>
+        <v>4.784349485562274</v>
       </c>
       <c r="Y2" t="n">
-        <v>13</v>
+        <v>124.1</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.7745966692414834</v>
+        <v>3.176476034853718</v>
       </c>
       <c r="AA2" t="n">
-        <v>13</v>
+        <v>124.8</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.7745966692414834</v>
+        <v>3.572114219898351</v>
       </c>
       <c r="AC2" t="n">
-        <v>13.4</v>
+        <v>123.5</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.2</v>
+        <v>4.129164564412516</v>
       </c>
       <c r="AE2" t="n">
-        <v>13.4</v>
+        <v>127.4</v>
       </c>
       <c r="AF2" t="n">
-        <v>1.42828568570857</v>
+        <v>3.006659275674582</v>
       </c>
       <c r="AG2" t="n">
-        <v>13.7</v>
+        <v>123.8</v>
       </c>
       <c r="AH2" t="n">
-        <v>1.1</v>
+        <v>5.134199061197374</v>
       </c>
       <c r="AI2" t="n">
-        <v>13.8</v>
+        <v>122.7</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1.077032961426901</v>
+        <v>3.551056180912941</v>
       </c>
       <c r="AK2" t="n">
-        <v>13.7</v>
+        <v>121.9</v>
       </c>
       <c r="AL2" t="n">
-        <v>1.268857754044952</v>
+        <v>3.448187929913333</v>
       </c>
       <c r="AM2" t="n">
-        <v>14.7</v>
+        <v>121.2</v>
       </c>
       <c r="AN2" t="n">
-        <v>1.187434208703792</v>
+        <v>4.833218389437829</v>
       </c>
       <c r="AO2" t="n">
-        <v>14.6</v>
+        <v>123.6</v>
       </c>
       <c r="AP2" t="n">
-        <v>1.113552872566004</v>
+        <v>5.730619512757761</v>
       </c>
       <c r="AQ2" t="n">
-        <v>14.2</v>
+        <v>122.6</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.8717797887081347</v>
+        <v>6.755738301621815</v>
       </c>
       <c r="AS2" t="n">
-        <v>15.5</v>
+        <v>124.5</v>
       </c>
       <c r="AT2" t="n">
-        <v>0.9219544457292888</v>
+        <v>5.142956348249516</v>
       </c>
       <c r="AU2" t="n">
-        <v>14.8</v>
+        <v>123.4</v>
       </c>
       <c r="AV2" t="n">
-        <v>0.7483314773547883</v>
+        <v>5.834380858325929</v>
       </c>
       <c r="AW2" t="n">
-        <v>15.6</v>
+        <v>121.9</v>
       </c>
       <c r="AX2" t="n">
-        <v>1.113552872566004</v>
+        <v>7.147726911403373</v>
       </c>
       <c r="AY2" t="n">
-        <v>16</v>
+        <v>122.3</v>
       </c>
       <c r="AZ2" t="n">
-        <v>1</v>
+        <v>8.626123115281858</v>
       </c>
       <c r="BA2" t="n">
-        <v>17</v>
+        <v>117.1</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.7745966692414834</v>
+        <v>3.83275357934736</v>
       </c>
       <c r="BC2" t="n">
-        <v>16.7</v>
+        <v>119.7</v>
       </c>
       <c r="BD2" t="n">
-        <v>1.268857754044952</v>
+        <v>7.071774883294858</v>
       </c>
       <c r="BE2" t="n">
-        <v>16.1</v>
+        <v>121.3</v>
       </c>
       <c r="BF2" t="n">
-        <v>1.513274595042156</v>
+        <v>9.121951545584968</v>
       </c>
       <c r="BG2" t="n">
-        <v>17.8</v>
+        <v>121.6</v>
       </c>
       <c r="BH2" t="n">
-        <v>1.077032961426901</v>
+        <v>10.32666451474047</v>
       </c>
       <c r="BI2" t="n">
-        <v>490.4</v>
+        <v>3774.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>